<commit_message>
Update IPCse - Series históricas.xlsx
</commit_message>
<xml_diff>
--- a/assets/excel/IPCse - Series históricas.xlsx
+++ b/assets/excel/IPCse - Series históricas.xlsx
@@ -1215,11 +1215,11 @@
   <dimension ref="B1:V89"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="78" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomRight" activeCell="E64" sqref="E64"/>
+      <selection pane="bottomRight" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update 07-24 + navi
</commit_message>
<xml_diff>
--- a/assets/excel/IPCse - Series históricas.xlsx
+++ b/assets/excel/IPCse - Series históricas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fiona\Dropbox\MGR\IPC seasonal adjustment\IPCse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70B35E1-16A6-47E1-A520-E2BDD7C4FD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A54FC34-2E8C-4F01-ACB9-8F6784DDFCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10416" yWindow="17172" windowWidth="30936" windowHeight="18696" activeTab="2" xr2:uid="{A81B6F3A-9175-42CA-B78F-287A4E3C6249}"/>
+    <workbookView xWindow="624" yWindow="636" windowWidth="23040" windowHeight="13608" activeTab="2" xr2:uid="{A81B6F3A-9175-42CA-B78F-287A4E3C6249}"/>
   </bookViews>
   <sheets>
     <sheet name="Índices" sheetId="1" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>IPCse NACIONAL</t>
   </si>
   <si>
-    <t>Ene.</t>
-  </si>
-  <si>
     <t>Feb.</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Jun.</t>
+  </si>
+  <si>
+    <t>Jul.</t>
   </si>
 </sst>
 </file>
@@ -1243,27 +1243,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA821952-0137-4F39-844C-15CA99AC928E}">
-  <dimension ref="B1:V95"/>
+  <dimension ref="B1:V96"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="78" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomRight" activeCell="G78" sqref="G78:G80"/>
+      <selection pane="bottomRight" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5703125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5546875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="4" customWidth="1"/>
-    <col min="2" max="3" width="20.5703125" style="4" customWidth="1"/>
-    <col min="4" max="21" width="15.5703125" style="4"/>
-    <col min="22" max="22" width="20.5703125" style="4" customWidth="1"/>
-    <col min="23" max="16384" width="15.5703125" style="4"/>
+    <col min="1" max="1" width="4.5546875" style="4" customWidth="1"/>
+    <col min="2" max="3" width="20.5546875" style="4" customWidth="1"/>
+    <col min="4" max="21" width="15.5546875" style="4"/>
+    <col min="22" max="22" width="20.5546875" style="4" customWidth="1"/>
+    <col min="23" max="16384" width="15.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="52" t="s">
         <v>10</v>
       </c>
@@ -1288,7 +1288,7 @@
       <c r="U2" s="53"/>
       <c r="V2" s="53"/>
     </row>
-    <row r="3" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
         <v>8</v>
@@ -1319,7 +1319,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:22" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:22" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B5" s="9">
         <v>42705</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>99.977400000000003</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
         <v>42736</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>101.58410000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B7" s="13">
         <v>42767</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>103.26909999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
         <v>42795</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>104.8601</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <v>42826</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>107.3261</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
         <v>42856</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>109.36450000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" s="13">
         <v>42887</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>110.7693</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
         <v>42917</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>112.8707</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B13" s="13">
         <v>42948</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>114.20829999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B14" s="13">
         <v>42979</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>115.16679999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B15" s="13">
         <v>43009</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>116.4616</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" s="13">
         <v>43040</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>118.2471</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="13">
         <v>43070</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>120.15</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
         <v>43101</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>122.66079999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="13">
         <v>43132</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>124.86669999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
         <v>43160</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>127.12269999999999</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
         <v>43191</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>129.41149999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="13">
         <v>43221</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>133.31610000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
         <v>43252</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>138.48570000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24" s="13">
         <v>43282</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>143.6498</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="13">
         <v>43313</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>148.0249</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26" s="13">
         <v>43344</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>157.21270000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="13">
         <v>43374</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>163.8939</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="13">
         <v>43405</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>169.81559999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="13">
         <v>43435</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>173.93020000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="13">
         <v>43466</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>179.21430000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31" s="13">
         <v>43497</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>186.506</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="13">
         <v>43525</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>194.3347</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B33" s="13">
         <v>43556</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>200.91579999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B34" s="13">
         <v>43586</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>207.03639999999999</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B35" s="13">
         <v>43617</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>212.8476</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B36" s="13">
         <v>43647</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>218.41489999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B37" s="13">
         <v>43678</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>227.71770000000001</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B38" s="13">
         <v>43709</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>240.4811</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B39" s="13">
         <v>43739</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>247.86199999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B40" s="13">
         <v>43770</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>259.3349</v>
       </c>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B41" s="13">
         <v>43800</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>268.79329999999999</v>
       </c>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B42" s="13">
         <v>43831</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>278.7826</v>
       </c>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B43" s="13">
         <v>43862</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>286.44729999999998</v>
       </c>
     </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B44" s="13">
         <v>43891</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>293.82990000000001</v>
       </c>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B45" s="13">
         <v>43922</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>300.18740000000003</v>
       </c>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B46" s="13">
         <v>43952</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>307.81490000000002</v>
       </c>
     </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B47" s="13">
         <v>43983</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>316.56420000000003</v>
       </c>
     </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B48" s="13">
         <v>44013</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>324.54230000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B49" s="13">
         <v>44044</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>333.78789999999998</v>
       </c>
     </row>
-    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B50" s="13">
         <v>44075</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>340.72519999999997</v>
       </c>
     </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B51" s="13">
         <v>44105</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>353.69189999999998</v>
       </c>
     </row>
-    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B52" s="13">
         <v>44136</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>367.19499999999999</v>
       </c>
     </row>
-    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B53" s="13">
         <v>44166</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>383.58569999999997</v>
       </c>
     </row>
-    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B54" s="13">
         <v>44197</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>400.52280000000002</v>
       </c>
     </row>
-    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B55" s="13">
         <v>44228</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>416.6268</v>
       </c>
     </row>
-    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B56" s="13">
         <v>44256</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>434.39139999999998</v>
       </c>
     </row>
-    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B57" s="13">
         <v>44287</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>451.8818</v>
       </c>
     </row>
-    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B58" s="13">
         <v>44317</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>467.42290000000003</v>
       </c>
     </row>
-    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B59" s="13">
         <v>44348</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>483.03149999999999</v>
       </c>
     </row>
-    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B60" s="13">
         <v>44378</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>499.71620000000001</v>
       </c>
     </row>
-    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B61" s="13">
         <v>44409</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>511.17930000000001</v>
       </c>
     </row>
-    <row r="62" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B62" s="13">
         <v>44440</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>525.85019999999997</v>
       </c>
     </row>
-    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B63" s="13">
         <v>44470</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>542.82629999999995</v>
       </c>
     </row>
-    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B64" s="13">
         <v>44501</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>560.64739999999995</v>
       </c>
     </row>
-    <row r="65" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B65" s="13">
         <v>44531</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>587.63199999999995</v>
       </c>
     </row>
-    <row r="66" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B66" s="13">
         <v>44562</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>614.96839999999997</v>
       </c>
     </row>
-    <row r="67" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B67" s="13">
         <v>44593</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>648.68989999999997</v>
       </c>
     </row>
-    <row r="68" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B68" s="13">
         <v>44621</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>686.36180000000002</v>
       </c>
     </row>
-    <row r="69" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B69" s="13">
         <v>44652</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>729.43140000000005</v>
       </c>
     </row>
-    <row r="70" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B70" s="13">
         <v>44682</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>770.00469999999996</v>
       </c>
     </row>
-    <row r="71" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B71" s="13">
         <v>44713</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>811.8424</v>
       </c>
     </row>
-    <row r="72" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B72" s="13">
         <v>44743</v>
       </c>
@@ -5804,7 +5804,7 @@
         <v>880.58450000000005</v>
       </c>
     </row>
-    <row r="73" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B73" s="13">
         <v>44774</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>944.6404</v>
       </c>
     </row>
-    <row r="74" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B74" s="13">
         <v>44805</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>1001.7683</v>
       </c>
     </row>
-    <row r="75" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B75" s="13">
         <v>44835</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>1059.6804</v>
       </c>
     </row>
-    <row r="76" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B76" s="13">
         <v>44866</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>1113.1264000000001</v>
       </c>
     </row>
-    <row r="77" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B77" s="13">
         <v>44896</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>1173.7402999999999</v>
       </c>
     </row>
-    <row r="78" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B78" s="13">
         <v>44927</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>1250.2503999999999</v>
       </c>
     </row>
-    <row r="79" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B79" s="13">
         <v>44958</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>1345.6905999999999</v>
       </c>
     </row>
-    <row r="80" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B80" s="13">
         <v>44986</v>
       </c>
@@ -6324,7 +6324,7 @@
         <v>1441.3485000000001</v>
       </c>
     </row>
-    <row r="81" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B81" s="13">
         <v>45017</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>1572.9845</v>
       </c>
     </row>
-    <row r="82" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B82" s="13">
         <v>45047</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>1696.7299</v>
       </c>
     </row>
-    <row r="83" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B83" s="13">
         <v>45078</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>1788.9819</v>
       </c>
     </row>
-    <row r="84" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B84" s="13">
         <v>45108</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>1904.9344000000001</v>
       </c>
     </row>
-    <row r="85" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B85" s="13">
         <v>45139</v>
       </c>
@@ -6649,7 +6649,7 @@
         <v>2149.5119</v>
       </c>
     </row>
-    <row r="86" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B86" s="13">
         <v>45170</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>2433.0675999999999</v>
       </c>
     </row>
-    <row r="87" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B87" s="13">
         <v>45200</v>
       </c>
@@ -6779,7 +6779,7 @@
         <v>2637.0823</v>
       </c>
     </row>
-    <row r="88" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B88" s="13">
         <v>45231</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>3008.4508000000001</v>
       </c>
     </row>
-    <row r="89" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B89" s="13">
         <v>45261</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>3793.6828</v>
       </c>
     </row>
-    <row r="90" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B90" s="13">
         <v>45292</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>4582.4724999999999</v>
       </c>
     </row>
-    <row r="91" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B91" s="13">
         <v>45323</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>5099.6557000000003</v>
       </c>
     </row>
-    <row r="92" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B92" s="13">
         <v>45352</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>5537.8856999999998</v>
       </c>
     </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B93" s="13">
         <v>45383</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>5906.4143999999997</v>
       </c>
     </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B94" s="13">
         <v>45413</v>
       </c>
@@ -7234,69 +7234,134 @@
         <v>6213.4395999999997</v>
       </c>
     </row>
-    <row r="95" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="14">
+    <row r="95" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B95" s="13">
         <v>45444</v>
       </c>
-      <c r="C95" s="18">
+      <c r="C95" s="15">
         <v>6371.3901999999998</v>
       </c>
-      <c r="D95" s="19">
+      <c r="D95" s="16">
         <v>6313.5257000000001</v>
       </c>
-      <c r="E95" s="19">
+      <c r="E95" s="16">
         <v>6415.5124999999998</v>
       </c>
-      <c r="F95" s="19">
+      <c r="F95" s="16">
         <v>6390.4237000000003</v>
       </c>
-      <c r="G95" s="19">
+      <c r="G95" s="16">
         <v>6420.165</v>
       </c>
-      <c r="H95" s="19">
+      <c r="H95" s="16">
         <v>6477.3638000000001</v>
       </c>
-      <c r="I95" s="20">
+      <c r="I95" s="17">
         <v>6264.3185999999996</v>
       </c>
-      <c r="J95" s="19">
+      <c r="J95" s="16">
         <v>7146.6593999999996</v>
       </c>
-      <c r="K95" s="19">
+      <c r="K95" s="16">
         <v>4914.8936000000003</v>
       </c>
-      <c r="L95" s="19">
+      <c r="L95" s="16">
         <v>5731.8341</v>
       </c>
-      <c r="M95" s="19">
+      <c r="M95" s="16">
         <v>5285.0308000000005</v>
       </c>
-      <c r="N95" s="19">
+      <c r="N95" s="16">
         <v>6107.6014999999998</v>
       </c>
-      <c r="O95" s="19">
+      <c r="O95" s="16">
         <v>7139.3881000000001</v>
       </c>
-      <c r="P95" s="19">
+      <c r="P95" s="16">
         <v>6816.393</v>
       </c>
-      <c r="Q95" s="19">
+      <c r="Q95" s="16">
         <v>5640.9961000000003</v>
       </c>
-      <c r="R95" s="19">
+      <c r="R95" s="16">
         <v>5784.0231000000003</v>
       </c>
-      <c r="S95" s="19">
+      <c r="S95" s="16">
         <v>4414.6482999999998</v>
       </c>
-      <c r="T95" s="19">
+      <c r="T95" s="16">
         <v>6631.1608999999999</v>
       </c>
-      <c r="U95" s="20">
+      <c r="U95" s="17">
         <v>6335.2188999999998</v>
       </c>
-      <c r="V95" s="18">
+      <c r="V95" s="15">
         <v>6452.8719000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="14">
+        <v>45474</v>
+      </c>
+      <c r="C96" s="18">
+        <v>6638.8073000000004</v>
+      </c>
+      <c r="D96" s="19">
+        <v>6568.8379999999997</v>
+      </c>
+      <c r="E96" s="19">
+        <v>6688.0135</v>
+      </c>
+      <c r="F96" s="19">
+        <v>6639.5613999999996</v>
+      </c>
+      <c r="G96" s="19">
+        <v>6721.6724000000004</v>
+      </c>
+      <c r="H96" s="19">
+        <v>6782.4107999999997</v>
+      </c>
+      <c r="I96" s="20">
+        <v>6519.8887000000004</v>
+      </c>
+      <c r="J96" s="19">
+        <v>7414.0300999999999</v>
+      </c>
+      <c r="K96" s="19">
+        <v>5240.8603000000003</v>
+      </c>
+      <c r="L96" s="19">
+        <v>5867.4665000000005</v>
+      </c>
+      <c r="M96" s="19">
+        <v>5605.2803000000004</v>
+      </c>
+      <c r="N96" s="19">
+        <v>6279.5263999999997</v>
+      </c>
+      <c r="O96" s="19">
+        <v>7557.0290000000005</v>
+      </c>
+      <c r="P96" s="19">
+        <v>6995.6211000000003</v>
+      </c>
+      <c r="Q96" s="19">
+        <v>5864.5308999999997</v>
+      </c>
+      <c r="R96" s="19">
+        <v>6057.9207999999999</v>
+      </c>
+      <c r="S96" s="19">
+        <v>4597.3388999999997</v>
+      </c>
+      <c r="T96" s="19">
+        <v>7057.2272000000003</v>
+      </c>
+      <c r="U96" s="20">
+        <v>6554.3981999999996</v>
+      </c>
+      <c r="V96" s="18">
+        <v>6714.0612000000001</v>
       </c>
     </row>
   </sheetData>
@@ -7312,27 +7377,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED968B30-91AE-4BCD-9838-818BA334E48C}">
-  <dimension ref="B1:V95"/>
+  <dimension ref="B1:V96"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="83" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomRight" activeCell="C95" sqref="C95"/>
+      <selection pane="bottomRight" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5703125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5546875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="4" customWidth="1"/>
-    <col min="2" max="3" width="20.5703125" style="4" customWidth="1"/>
-    <col min="4" max="21" width="15.5703125" style="4"/>
-    <col min="22" max="22" width="20.5703125" style="4" customWidth="1"/>
-    <col min="23" max="16384" width="15.5703125" style="4"/>
+    <col min="1" max="1" width="4.5546875" style="4" customWidth="1"/>
+    <col min="2" max="3" width="20.5546875" style="4" customWidth="1"/>
+    <col min="4" max="21" width="15.5546875" style="4"/>
+    <col min="22" max="22" width="20.5546875" style="4" customWidth="1"/>
+    <col min="23" max="16384" width="15.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="52" t="s">
         <v>11</v>
       </c>
@@ -7357,7 +7422,7 @@
       <c r="U2" s="53"/>
       <c r="V2" s="53"/>
     </row>
-    <row r="3" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
         <v>8</v>
@@ -7388,7 +7453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:22" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:22" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -7453,7 +7518,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B5" s="9">
         <v>42705</v>
       </c>
@@ -7478,7 +7543,7 @@
       <c r="U5" s="12"/>
       <c r="V5" s="10"/>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
         <v>42736</v>
       </c>
@@ -7543,7 +7608,7 @@
         <v>1.6071</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B7" s="13">
         <v>42767</v>
       </c>
@@ -7608,7 +7673,7 @@
         <v>1.6587000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
         <v>42795</v>
       </c>
@@ -7673,7 +7738,7 @@
         <v>1.5406</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <v>42826</v>
       </c>
@@ -7738,7 +7803,7 @@
         <v>2.3517000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
         <v>42856</v>
       </c>
@@ -7803,7 +7868,7 @@
         <v>1.8993</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" s="13">
         <v>42887</v>
       </c>
@@ -7868,7 +7933,7 @@
         <v>1.2845</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
         <v>42917</v>
       </c>
@@ -7933,7 +7998,7 @@
         <v>1.8971</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B13" s="13">
         <v>42948</v>
       </c>
@@ -7998,7 +8063,7 @@
         <v>1.1851</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B14" s="13">
         <v>42979</v>
       </c>
@@ -8063,7 +8128,7 @@
         <v>0.83930000000000005</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B15" s="13">
         <v>43009</v>
       </c>
@@ -8128,7 +8193,7 @@
         <v>1.1243000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" s="13">
         <v>43040</v>
       </c>
@@ -8193,7 +8258,7 @@
         <v>1.5330999999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="13">
         <v>43070</v>
       </c>
@@ -8258,7 +8323,7 @@
         <v>1.6093</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
         <v>43101</v>
       </c>
@@ -8323,7 +8388,7 @@
         <v>2.0897000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="13">
         <v>43132</v>
       </c>
@@ -8388,7 +8453,7 @@
         <v>1.7984</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
         <v>43160</v>
       </c>
@@ -8453,7 +8518,7 @@
         <v>1.8067</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
         <v>43191</v>
       </c>
@@ -8518,7 +8583,7 @@
         <v>1.8005</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="13">
         <v>43221</v>
       </c>
@@ -8583,7 +8648,7 @@
         <v>3.0171999999999999</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
         <v>43252</v>
       </c>
@@ -8648,7 +8713,7 @@
         <v>3.8776999999999999</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24" s="13">
         <v>43282</v>
       </c>
@@ -8713,7 +8778,7 @@
         <v>3.7290000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="13">
         <v>43313</v>
       </c>
@@ -8778,7 +8843,7 @@
         <v>3.0457000000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26" s="13">
         <v>43344</v>
       </c>
@@ -8843,7 +8908,7 @@
         <v>6.2069000000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="13">
         <v>43374</v>
       </c>
@@ -8908,7 +8973,7 @@
         <v>4.2497999999999996</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="13">
         <v>43405</v>
       </c>
@@ -8973,7 +9038,7 @@
         <v>3.6131000000000002</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="13">
         <v>43435</v>
       </c>
@@ -9038,7 +9103,7 @@
         <v>2.423</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="13">
         <v>43466</v>
       </c>
@@ -9103,7 +9168,7 @@
         <v>3.0381</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31" s="13">
         <v>43497</v>
       </c>
@@ -9168,7 +9233,7 @@
         <v>4.0686999999999998</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="13">
         <v>43525</v>
       </c>
@@ -9233,7 +9298,7 @@
         <v>4.1976000000000004</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B33" s="13">
         <v>43556</v>
       </c>
@@ -9298,7 +9363,7 @@
         <v>3.3864999999999998</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B34" s="13">
         <v>43586</v>
       </c>
@@ -9363,7 +9428,7 @@
         <v>3.0464000000000002</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B35" s="13">
         <v>43617</v>
       </c>
@@ -9428,7 +9493,7 @@
         <v>2.8068</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B36" s="13">
         <v>43647</v>
       </c>
@@ -9493,7 +9558,7 @@
         <v>2.6156000000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B37" s="13">
         <v>43678</v>
       </c>
@@ -9558,7 +9623,7 @@
         <v>4.2591999999999999</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B38" s="13">
         <v>43709</v>
       </c>
@@ -9623,7 +9688,7 @@
         <v>5.6048999999999998</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B39" s="13">
         <v>43739</v>
       </c>
@@ -9688,7 +9753,7 @@
         <v>3.0691999999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B40" s="13">
         <v>43770</v>
       </c>
@@ -9753,7 +9818,7 @@
         <v>4.6287000000000003</v>
       </c>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B41" s="13">
         <v>43800</v>
       </c>
@@ -9818,7 +9883,7 @@
         <v>3.6472000000000002</v>
       </c>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B42" s="13">
         <v>43831</v>
       </c>
@@ -9883,7 +9948,7 @@
         <v>3.7164000000000001</v>
       </c>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B43" s="13">
         <v>43862</v>
       </c>
@@ -9948,7 +10013,7 @@
         <v>2.7492999999999999</v>
       </c>
     </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B44" s="13">
         <v>43891</v>
       </c>
@@ -10013,7 +10078,7 @@
         <v>2.5773000000000001</v>
       </c>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B45" s="13">
         <v>43922</v>
       </c>
@@ -10078,7 +10143,7 @@
         <v>2.1637</v>
       </c>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B46" s="13">
         <v>43952</v>
       </c>
@@ -10143,7 +10208,7 @@
         <v>2.5409000000000002</v>
       </c>
     </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B47" s="13">
         <v>43983</v>
       </c>
@@ -10208,7 +10273,7 @@
         <v>2.8424</v>
       </c>
     </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B48" s="13">
         <v>44013</v>
       </c>
@@ -10273,7 +10338,7 @@
         <v>2.5202</v>
       </c>
     </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B49" s="13">
         <v>44044</v>
       </c>
@@ -10338,7 +10403,7 @@
         <v>2.8488000000000002</v>
       </c>
     </row>
-    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B50" s="13">
         <v>44075</v>
       </c>
@@ -10403,7 +10468,7 @@
         <v>2.0783999999999998</v>
       </c>
     </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B51" s="13">
         <v>44105</v>
       </c>
@@ -10468,7 +10533,7 @@
         <v>3.8056000000000001</v>
       </c>
     </row>
-    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B52" s="13">
         <v>44136</v>
       </c>
@@ -10533,7 +10598,7 @@
         <v>3.8178000000000001</v>
       </c>
     </row>
-    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B53" s="13">
         <v>44166</v>
       </c>
@@ -10598,7 +10663,7 @@
         <v>4.4638</v>
       </c>
     </row>
-    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B54" s="13">
         <v>44197</v>
       </c>
@@ -10663,7 +10728,7 @@
         <v>4.4154999999999998</v>
       </c>
     </row>
-    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B55" s="13">
         <v>44228</v>
       </c>
@@ -10728,7 +10793,7 @@
         <v>4.0206999999999997</v>
       </c>
     </row>
-    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B56" s="13">
         <v>44256</v>
       </c>
@@ -10793,7 +10858,7 @@
         <v>4.2638999999999996</v>
       </c>
     </row>
-    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B57" s="13">
         <v>44287</v>
       </c>
@@ -10858,7 +10923,7 @@
         <v>4.0263999999999998</v>
       </c>
     </row>
-    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B58" s="13">
         <v>44317</v>
       </c>
@@ -10923,7 +10988,7 @@
         <v>3.4392</v>
       </c>
     </row>
-    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B59" s="13">
         <v>44348</v>
       </c>
@@ -10988,7 +11053,7 @@
         <v>3.3393000000000002</v>
       </c>
     </row>
-    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B60" s="13">
         <v>44378</v>
       </c>
@@ -11053,7 +11118,7 @@
         <v>3.4542000000000002</v>
       </c>
     </row>
-    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B61" s="13">
         <v>44409</v>
       </c>
@@ -11118,7 +11183,7 @@
         <v>2.2938999999999998</v>
       </c>
     </row>
-    <row r="62" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B62" s="13">
         <v>44440</v>
       </c>
@@ -11183,7 +11248,7 @@
         <v>2.87</v>
       </c>
     </row>
-    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B63" s="13">
         <v>44470</v>
       </c>
@@ -11248,7 +11313,7 @@
         <v>3.2282999999999999</v>
       </c>
     </row>
-    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B64" s="13">
         <v>44501</v>
       </c>
@@ -11313,7 +11378,7 @@
         <v>3.2829999999999999</v>
       </c>
     </row>
-    <row r="65" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B65" s="13">
         <v>44531</v>
       </c>
@@ -11378,7 +11443,7 @@
         <v>4.8131000000000004</v>
       </c>
     </row>
-    <row r="66" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B66" s="13">
         <v>44562</v>
       </c>
@@ -11443,7 +11508,7 @@
         <v>4.6520000000000001</v>
       </c>
     </row>
-    <row r="67" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B67" s="13">
         <v>44593</v>
       </c>
@@ -11508,7 +11573,7 @@
         <v>5.4835000000000003</v>
       </c>
     </row>
-    <row r="68" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B68" s="13">
         <v>44621</v>
       </c>
@@ -11573,7 +11638,7 @@
         <v>5.8074000000000003</v>
       </c>
     </row>
-    <row r="69" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B69" s="13">
         <v>44652</v>
       </c>
@@ -11638,7 +11703,7 @@
         <v>6.2751000000000001</v>
       </c>
     </row>
-    <row r="70" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B70" s="13">
         <v>44682</v>
       </c>
@@ -11703,7 +11768,7 @@
         <v>5.5622999999999996</v>
       </c>
     </row>
-    <row r="71" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B71" s="13">
         <v>44713</v>
       </c>
@@ -11768,7 +11833,7 @@
         <v>5.4333999999999998</v>
       </c>
     </row>
-    <row r="72" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B72" s="13">
         <v>44743</v>
       </c>
@@ -11833,7 +11898,7 @@
         <v>8.4673999999999996</v>
       </c>
     </row>
-    <row r="73" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B73" s="13">
         <v>44774</v>
       </c>
@@ -11898,7 +11963,7 @@
         <v>7.2742000000000004</v>
       </c>
     </row>
-    <row r="74" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B74" s="13">
         <v>44805</v>
       </c>
@@ -11963,7 +12028,7 @@
         <v>6.0476000000000001</v>
       </c>
     </row>
-    <row r="75" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B75" s="13">
         <v>44835</v>
       </c>
@@ -12028,7 +12093,7 @@
         <v>5.7809999999999997</v>
       </c>
     </row>
-    <row r="76" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B76" s="13">
         <v>44866</v>
       </c>
@@ -12093,7 +12158,7 @@
         <v>5.0435999999999996</v>
       </c>
     </row>
-    <row r="77" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B77" s="13">
         <v>44896</v>
       </c>
@@ -12158,7 +12223,7 @@
         <v>5.4454000000000002</v>
       </c>
     </row>
-    <row r="78" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B78" s="13">
         <v>44927</v>
       </c>
@@ -12223,7 +12288,7 @@
         <v>6.5185000000000004</v>
       </c>
     </row>
-    <row r="79" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B79" s="13">
         <v>44958</v>
       </c>
@@ -12288,7 +12353,7 @@
         <v>7.6337000000000002</v>
       </c>
     </row>
-    <row r="80" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B80" s="13">
         <v>44986</v>
       </c>
@@ -12353,7 +12418,7 @@
         <v>7.1085000000000003</v>
       </c>
     </row>
-    <row r="81" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B81" s="13">
         <v>45017</v>
       </c>
@@ -12418,7 +12483,7 @@
         <v>9.1327999999999996</v>
       </c>
     </row>
-    <row r="82" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B82" s="13">
         <v>45047</v>
       </c>
@@ -12483,7 +12548,7 @@
         <v>7.8669000000000002</v>
       </c>
     </row>
-    <row r="83" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B83" s="13">
         <v>45078</v>
       </c>
@@ -12548,7 +12613,7 @@
         <v>5.4370000000000003</v>
       </c>
     </row>
-    <row r="84" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B84" s="13">
         <v>45108</v>
       </c>
@@ -12613,7 +12678,7 @@
         <v>6.4814999999999996</v>
       </c>
     </row>
-    <row r="85" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B85" s="13">
         <v>45139</v>
       </c>
@@ -12678,7 +12743,7 @@
         <v>12.8392</v>
       </c>
     </row>
-    <row r="86" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B86" s="13">
         <v>45170</v>
       </c>
@@ -12743,7 +12808,7 @@
         <v>13.191599999999999</v>
       </c>
     </row>
-    <row r="87" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B87" s="13">
         <v>45200</v>
       </c>
@@ -12808,7 +12873,7 @@
         <v>8.3850999999999996</v>
       </c>
     </row>
-    <row r="88" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B88" s="13">
         <v>45231</v>
       </c>
@@ -12873,7 +12938,7 @@
         <v>14.082599999999999</v>
       </c>
     </row>
-    <row r="89" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B89" s="13">
         <v>45261</v>
       </c>
@@ -12938,7 +13003,7 @@
         <v>26.100899999999999</v>
       </c>
     </row>
-    <row r="90" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B90" s="13">
         <v>45292</v>
       </c>
@@ -13003,7 +13068,7 @@
         <v>20.792200000000001</v>
       </c>
     </row>
-    <row r="91" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B91" s="13">
         <v>45323</v>
       </c>
@@ -13068,7 +13133,7 @@
         <v>11.286099999999999</v>
       </c>
     </row>
-    <row r="92" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B92" s="13">
         <v>45352</v>
       </c>
@@ -13133,7 +13198,7 @@
         <v>8.5932999999999993</v>
       </c>
     </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B93" s="13">
         <v>45383</v>
       </c>
@@ -13198,7 +13263,7 @@
         <v>6.6547000000000001</v>
       </c>
     </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B94" s="13">
         <v>45413</v>
       </c>
@@ -13263,69 +13328,134 @@
         <v>5.1981999999999999</v>
       </c>
     </row>
-    <row r="95" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="48">
+    <row r="95" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B95" s="13">
         <v>45444</v>
       </c>
-      <c r="C95" s="18">
+      <c r="C95" s="15">
         <v>4.7572999999999999</v>
       </c>
-      <c r="D95" s="19">
+      <c r="D95" s="16">
         <v>4.5137999999999998</v>
       </c>
-      <c r="E95" s="19">
+      <c r="E95" s="16">
         <v>5.0039999999999996</v>
       </c>
-      <c r="F95" s="19">
+      <c r="F95" s="16">
         <v>5.0018000000000002</v>
       </c>
-      <c r="G95" s="19">
+      <c r="G95" s="16">
         <v>4.7289000000000003</v>
       </c>
-      <c r="H95" s="19">
+      <c r="H95" s="16">
         <v>5.1580000000000004</v>
       </c>
-      <c r="I95" s="20">
+      <c r="I95" s="17">
         <v>5.0720999999999998</v>
       </c>
-      <c r="J95" s="19">
+      <c r="J95" s="16">
         <v>3.5796000000000001</v>
       </c>
-      <c r="K95" s="19">
+      <c r="K95" s="16">
         <v>1.9865999999999999</v>
       </c>
-      <c r="L95" s="19">
+      <c r="L95" s="16">
         <v>2.9434</v>
       </c>
-      <c r="M95" s="19">
+      <c r="M95" s="16">
         <v>14.4078</v>
       </c>
-      <c r="N95" s="19">
+      <c r="N95" s="16">
         <v>1.8645</v>
       </c>
-      <c r="O95" s="19">
+      <c r="O95" s="16">
         <v>4.7492000000000001</v>
       </c>
-      <c r="P95" s="19">
+      <c r="P95" s="16">
         <v>3.9338000000000002</v>
       </c>
-      <c r="Q95" s="19">
+      <c r="Q95" s="16">
         <v>5.2653999999999996</v>
       </c>
-      <c r="R95" s="19">
+      <c r="R95" s="16">
         <v>5.5656999999999996</v>
       </c>
-      <c r="S95" s="19">
+      <c r="S95" s="16">
         <v>8.3085000000000004</v>
       </c>
-      <c r="T95" s="19">
+      <c r="T95" s="16">
         <v>6.3105000000000002</v>
       </c>
-      <c r="U95" s="20">
+      <c r="U95" s="17">
         <v>2.7564000000000002</v>
       </c>
-      <c r="V95" s="18">
+      <c r="V95" s="15">
         <v>3.8534999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="48">
+        <v>45474</v>
+      </c>
+      <c r="C96" s="18">
+        <v>4.1971999999999996</v>
+      </c>
+      <c r="D96" s="19">
+        <v>4.0438999999999998</v>
+      </c>
+      <c r="E96" s="19">
+        <v>4.2474999999999996</v>
+      </c>
+      <c r="F96" s="19">
+        <v>3.8986000000000001</v>
+      </c>
+      <c r="G96" s="19">
+        <v>4.6962999999999999</v>
+      </c>
+      <c r="H96" s="19">
+        <v>4.7093999999999996</v>
+      </c>
+      <c r="I96" s="20">
+        <v>4.0797999999999996</v>
+      </c>
+      <c r="J96" s="19">
+        <v>3.7412000000000001</v>
+      </c>
+      <c r="K96" s="19">
+        <v>6.6322000000000001</v>
+      </c>
+      <c r="L96" s="19">
+        <v>2.3662999999999998</v>
+      </c>
+      <c r="M96" s="19">
+        <v>6.0595999999999997</v>
+      </c>
+      <c r="N96" s="19">
+        <v>2.8149000000000002</v>
+      </c>
+      <c r="O96" s="19">
+        <v>5.8498000000000001</v>
+      </c>
+      <c r="P96" s="19">
+        <v>2.6294</v>
+      </c>
+      <c r="Q96" s="19">
+        <v>3.9626999999999999</v>
+      </c>
+      <c r="R96" s="19">
+        <v>4.7354000000000003</v>
+      </c>
+      <c r="S96" s="19">
+        <v>4.1383000000000001</v>
+      </c>
+      <c r="T96" s="19">
+        <v>6.4252000000000002</v>
+      </c>
+      <c r="U96" s="20">
+        <v>3.4597000000000002</v>
+      </c>
+      <c r="V96" s="18">
+        <v>4.0476000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -13343,17 +13473,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83293D6D-81C8-49B2-8C10-806B04E884B0}">
   <dimension ref="B1:I39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="116" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="50.5703125" customWidth="1"/>
-    <col min="3" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" customWidth="1"/>
+    <col min="3" max="8" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="55" t="s">
         <v>13</v>
       </c>
@@ -13365,7 +13497,7 @@
       <c r="H2" s="56"/>
       <c r="I2" s="57"/>
     </row>
-    <row r="3" spans="2:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="22" t="s">
         <v>14</v>
       </c>
@@ -13381,12 +13513,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="65">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D4" s="65"/>
       <c r="E4" s="65"/>
@@ -13395,10 +13527,10 @@
       <c r="H4" s="65"/>
       <c r="I4" s="23" t="str">
         <f>+_xlfn.CONCAT(H5, " ", C4, "/", H5, " ", C4-1)</f>
-        <v>Jun. 2023/Jun. 2022</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <v>Jul. 2024/Jul. 2023</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="24"/>
       <c r="C5" s="25" t="s">
         <v>40</v>
@@ -13420,33 +13552,33 @@
       </c>
       <c r="I5" s="47"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="27">
-        <v>20.7379</v>
+        <v>13.4008</v>
       </c>
       <c r="D6" s="27">
-        <v>13.4008</v>
+        <v>10.164400000000001</v>
       </c>
       <c r="E6" s="27">
-        <v>10.164400000000001</v>
+        <v>8.7431999999999999</v>
       </c>
       <c r="F6" s="27">
-        <v>8.7431999999999999</v>
+        <v>4.5728999999999997</v>
       </c>
       <c r="G6" s="27">
-        <v>4.5728999999999997</v>
+        <v>4.7572999999999999</v>
       </c>
       <c r="H6" s="27">
-        <v>4.7572999999999999</v>
+        <v>4.1971999999999996</v>
       </c>
       <c r="I6" s="28">
-        <v>271.52969999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>263.44569999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="59" t="s">
         <v>7</v>
       </c>
@@ -13458,163 +13590,163 @@
       <c r="H7" s="60"/>
       <c r="I7" s="61"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="32">
-        <v>19.487200000000001</v>
+        <v>15.286</v>
       </c>
       <c r="D8" s="32">
-        <v>15.286</v>
+        <v>10.3573</v>
       </c>
       <c r="E8" s="32">
-        <v>10.3573</v>
+        <v>9.1841000000000008</v>
       </c>
       <c r="F8" s="32">
-        <v>9.1841000000000008</v>
+        <v>4.7674000000000003</v>
       </c>
       <c r="G8" s="32">
-        <v>4.7674000000000003</v>
+        <v>4.5137999999999998</v>
       </c>
       <c r="H8" s="32">
-        <v>4.5137999999999998</v>
+        <v>4.0438999999999998</v>
       </c>
       <c r="I8" s="33">
-        <v>273.67910000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+        <v>266.11270000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="32">
-        <v>21.381399999999999</v>
+        <v>11.950900000000001</v>
       </c>
       <c r="D9" s="32">
-        <v>11.950900000000001</v>
+        <v>10.5008</v>
       </c>
       <c r="E9" s="32">
-        <v>10.5008</v>
+        <v>8.6998999999999995</v>
       </c>
       <c r="F9" s="32">
-        <v>8.6998999999999995</v>
+        <v>4.3362999999999996</v>
       </c>
       <c r="G9" s="32">
-        <v>4.3362999999999996</v>
+        <v>5.0039999999999996</v>
       </c>
       <c r="H9" s="32">
-        <v>5.0039999999999996</v>
+        <v>4.2474999999999996</v>
       </c>
       <c r="I9" s="33">
-        <v>271.63900000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>262.89229999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="32">
-        <v>21.819099999999999</v>
+        <v>11.765000000000001</v>
       </c>
       <c r="D10" s="32">
-        <v>11.765000000000001</v>
+        <v>8.0137999999999998</v>
       </c>
       <c r="E10" s="32">
-        <v>8.0137999999999998</v>
+        <v>9.0043000000000006</v>
       </c>
       <c r="F10" s="32">
-        <v>9.0043000000000006</v>
+        <v>4.5412999999999997</v>
       </c>
       <c r="G10" s="32">
-        <v>4.5412999999999997</v>
+        <v>5.0018000000000002</v>
       </c>
       <c r="H10" s="32">
-        <v>5.0018000000000002</v>
+        <v>3.8986000000000001</v>
       </c>
       <c r="I10" s="33">
-        <v>262.37830000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <v>253.87440000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="32">
-        <v>19.981400000000001</v>
+        <v>10.963900000000001</v>
       </c>
       <c r="D11" s="32">
-        <v>10.963900000000001</v>
+        <v>10.056800000000001</v>
       </c>
       <c r="E11" s="32">
-        <v>10.056800000000001</v>
+        <v>6.3064999999999998</v>
       </c>
       <c r="F11" s="32">
-        <v>6.3064999999999998</v>
+        <v>4.1321000000000003</v>
       </c>
       <c r="G11" s="32">
-        <v>4.1321000000000003</v>
+        <v>4.7289000000000003</v>
       </c>
       <c r="H11" s="32">
-        <v>4.7289000000000003</v>
+        <v>4.6962999999999999</v>
       </c>
       <c r="I11" s="33">
-        <v>258.69819999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+        <v>253.12039999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="31" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="32">
-        <v>22.540900000000001</v>
+        <v>13.427899999999999</v>
       </c>
       <c r="D12" s="32">
-        <v>13.427899999999999</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="E12" s="32">
-        <v>8.7100000000000009</v>
+        <v>8.0625</v>
       </c>
       <c r="F12" s="32">
-        <v>8.0625</v>
+        <v>4.6234999999999999</v>
       </c>
       <c r="G12" s="32">
-        <v>4.6234999999999999</v>
+        <v>5.1580000000000004</v>
       </c>
       <c r="H12" s="32">
-        <v>5.1580000000000004</v>
+        <v>4.7093999999999996</v>
       </c>
       <c r="I12" s="33">
-        <v>271.86020000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>265.8569</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="31" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="32">
-        <v>24.8538</v>
+        <v>11.549300000000001</v>
       </c>
       <c r="D13" s="32">
-        <v>11.549300000000001</v>
+        <v>9.9405999999999999</v>
       </c>
       <c r="E13" s="32">
-        <v>9.9405999999999999</v>
+        <v>8.4405000000000001</v>
       </c>
       <c r="F13" s="32">
-        <v>8.4405000000000001</v>
+        <v>4.8232999999999997</v>
       </c>
       <c r="G13" s="32">
-        <v>4.8232999999999997</v>
+        <v>5.0720999999999998</v>
       </c>
       <c r="H13" s="32">
-        <v>5.0720999999999998</v>
+        <v>4.0797999999999996</v>
       </c>
       <c r="I13" s="33">
-        <v>276.87759999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>264.16149999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="31"/>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
@@ -13624,7 +13756,7 @@
       <c r="H14" s="32"/>
       <c r="I14" s="33"/>
     </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="62" t="s">
         <v>9</v>
       </c>
@@ -13636,319 +13768,319 @@
       <c r="H15" s="63"/>
       <c r="I15" s="64"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="32">
-        <v>20.2986</v>
+        <v>11.379200000000001</v>
       </c>
       <c r="D16" s="32">
-        <v>11.379200000000001</v>
+        <v>9.5661000000000005</v>
       </c>
       <c r="E16" s="32">
-        <v>9.5661000000000005</v>
+        <v>6.1928000000000001</v>
       </c>
       <c r="F16" s="32">
-        <v>6.1928000000000001</v>
+        <v>5.7142999999999997</v>
       </c>
       <c r="G16" s="32">
-        <v>5.7142999999999997</v>
+        <v>3.5796000000000001</v>
       </c>
       <c r="H16" s="32">
-        <v>3.5796000000000001</v>
+        <v>3.7412000000000001</v>
       </c>
       <c r="I16" s="33">
-        <v>285.12419999999997</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+        <v>275.81830000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="32">
-        <v>21.049499999999998</v>
+        <v>18.6081</v>
       </c>
       <c r="D17" s="32">
-        <v>18.6081</v>
+        <v>11.4427</v>
       </c>
       <c r="E17" s="32">
-        <v>11.4427</v>
+        <v>6.5521000000000003</v>
       </c>
       <c r="F17" s="32">
-        <v>6.5521000000000003</v>
+        <v>7.3403</v>
       </c>
       <c r="G17" s="32">
-        <v>7.3403</v>
+        <v>1.9865999999999999</v>
       </c>
       <c r="H17" s="32">
-        <v>1.9865999999999999</v>
+        <v>6.6322000000000001</v>
       </c>
       <c r="I17" s="33">
-        <v>257.73540000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+        <v>248.1456</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="32">
-        <v>13.392300000000001</v>
+        <v>9.5421999999999993</v>
       </c>
       <c r="D18" s="32">
-        <v>9.5421999999999993</v>
+        <v>6.9301000000000004</v>
       </c>
       <c r="E18" s="32">
-        <v>6.9301000000000004</v>
+        <v>7.2812000000000001</v>
       </c>
       <c r="F18" s="32">
-        <v>7.2812000000000001</v>
+        <v>4.4522000000000004</v>
       </c>
       <c r="G18" s="32">
-        <v>4.4522000000000004</v>
+        <v>2.9434</v>
       </c>
       <c r="H18" s="32">
-        <v>2.9434</v>
+        <v>2.3662999999999998</v>
       </c>
       <c r="I18" s="33">
-        <v>189.2054</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+        <v>185.2474</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="31" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="32">
-        <v>14.2448</v>
+        <v>20.098299999999998</v>
       </c>
       <c r="D19" s="32">
-        <v>20.098299999999998</v>
+        <v>13.2197</v>
       </c>
       <c r="E19" s="32">
-        <v>13.2197</v>
+        <v>35.386299999999999</v>
       </c>
       <c r="F19" s="32">
-        <v>35.386299999999999</v>
+        <v>2.5518000000000001</v>
       </c>
       <c r="G19" s="32">
-        <v>2.5518000000000001</v>
+        <v>14.4078</v>
       </c>
       <c r="H19" s="32">
-        <v>14.4078</v>
+        <v>6.0595999999999997</v>
       </c>
       <c r="I19" s="33">
-        <v>298.86689999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+        <v>306.61880000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="32">
-        <v>22.438099999999999</v>
+        <v>10.5862</v>
       </c>
       <c r="D20" s="32">
-        <v>10.5862</v>
+        <v>5.1493000000000002</v>
       </c>
       <c r="E20" s="32">
-        <v>5.1493000000000002</v>
+        <v>6.7298999999999998</v>
       </c>
       <c r="F20" s="32">
-        <v>6.7298999999999998</v>
+        <v>3.46</v>
       </c>
       <c r="G20" s="32">
-        <v>3.46</v>
+        <v>1.8645</v>
       </c>
       <c r="H20" s="32">
-        <v>1.8645</v>
+        <v>2.8149000000000002</v>
       </c>
       <c r="I20" s="33">
-        <v>253.6651</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+        <v>244.66159999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="31" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="32">
-        <v>20.499500000000001</v>
+        <v>13.5733</v>
       </c>
       <c r="D21" s="32">
-        <v>13.5733</v>
+        <v>12.2319</v>
       </c>
       <c r="E21" s="32">
-        <v>12.2319</v>
+        <v>9.1309000000000005</v>
       </c>
       <c r="F21" s="32">
-        <v>9.1309000000000005</v>
+        <v>0.69</v>
       </c>
       <c r="G21" s="32">
-        <v>0.69</v>
+        <v>4.7492000000000001</v>
       </c>
       <c r="H21" s="32">
-        <v>4.7492000000000001</v>
+        <v>5.8498000000000001</v>
       </c>
       <c r="I21" s="33">
-        <v>292.79180000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+        <v>281.32909999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="32">
-        <v>26.314499999999999</v>
+        <v>21.3124</v>
       </c>
       <c r="D22" s="32">
-        <v>21.3124</v>
+        <v>12.997999999999999</v>
       </c>
       <c r="E22" s="32">
-        <v>12.997999999999999</v>
+        <v>6.2891000000000004</v>
       </c>
       <c r="F22" s="32">
-        <v>6.2891000000000004</v>
+        <v>3.9729000000000001</v>
       </c>
       <c r="G22" s="32">
-        <v>3.9729000000000001</v>
+        <v>3.9338000000000002</v>
       </c>
       <c r="H22" s="32">
-        <v>3.9338000000000002</v>
+        <v>2.6294</v>
       </c>
       <c r="I22" s="33">
-        <v>299.67439999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+        <v>289.50560000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="31" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="32">
-        <v>23.994299999999999</v>
+        <v>24.742799999999999</v>
       </c>
       <c r="D23" s="32">
-        <v>24.742799999999999</v>
+        <v>15.887</v>
       </c>
       <c r="E23" s="32">
-        <v>15.887</v>
+        <v>14.7713</v>
       </c>
       <c r="F23" s="32">
-        <v>14.7713</v>
+        <v>8.6944999999999997</v>
       </c>
       <c r="G23" s="32">
-        <v>8.6944999999999997</v>
+        <v>5.2653999999999996</v>
       </c>
       <c r="H23" s="32">
-        <v>5.2653999999999996</v>
+        <v>3.9626999999999999</v>
       </c>
       <c r="I23" s="33">
-        <v>353.42090000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+        <v>318.54559999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="31" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="32">
-        <v>24.026</v>
+        <v>9.5474999999999994</v>
       </c>
       <c r="D24" s="32">
-        <v>9.5474999999999994</v>
+        <v>9.0190000000000001</v>
       </c>
       <c r="E24" s="32">
-        <v>9.0190000000000001</v>
+        <v>7.3421000000000003</v>
       </c>
       <c r="F24" s="32">
-        <v>7.3421000000000003</v>
+        <v>4.5571000000000002</v>
       </c>
       <c r="G24" s="32">
-        <v>4.5571000000000002</v>
+        <v>5.5656999999999996</v>
       </c>
       <c r="H24" s="32">
-        <v>5.5656999999999996</v>
+        <v>4.7354000000000003</v>
       </c>
       <c r="I24" s="33">
-        <v>267.1771</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+        <v>248.93469999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="31" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="32">
-        <v>2.3591000000000002</v>
+        <v>11.2354</v>
       </c>
       <c r="D25" s="32">
-        <v>11.2354</v>
+        <v>29.938800000000001</v>
       </c>
       <c r="E25" s="32">
-        <v>29.938800000000001</v>
+        <v>10.162800000000001</v>
       </c>
       <c r="F25" s="32">
-        <v>10.162800000000001</v>
+        <v>8.6125000000000007</v>
       </c>
       <c r="G25" s="32">
-        <v>8.6125000000000007</v>
+        <v>8.3085000000000004</v>
       </c>
       <c r="H25" s="32">
-        <v>8.3085000000000004</v>
+        <v>4.1383000000000001</v>
       </c>
       <c r="I25" s="33">
-        <v>220.0942</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+        <v>214.24850000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="32">
-        <v>19.302700000000002</v>
+        <v>11.1287</v>
       </c>
       <c r="D26" s="32">
-        <v>11.1287</v>
+        <v>8.3148</v>
       </c>
       <c r="E26" s="32">
-        <v>8.3148</v>
+        <v>7.2893999999999997</v>
       </c>
       <c r="F26" s="32">
-        <v>7.2893999999999997</v>
+        <v>5.5715000000000003</v>
       </c>
       <c r="G26" s="32">
-        <v>5.5715000000000003</v>
+        <v>6.3105000000000002</v>
       </c>
       <c r="H26" s="32">
-        <v>6.3105000000000002</v>
+        <v>6.4252000000000002</v>
       </c>
       <c r="I26" s="33">
-        <v>250.91</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+        <v>247.6943</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="32">
-        <v>44.463900000000002</v>
+        <v>16.633199999999999</v>
       </c>
       <c r="D27" s="32">
-        <v>16.633199999999999</v>
+        <v>9.6061999999999994</v>
       </c>
       <c r="E27" s="32">
-        <v>9.6061999999999994</v>
+        <v>5.7464000000000004</v>
       </c>
       <c r="F27" s="32">
-        <v>5.7464000000000004</v>
+        <v>4.3890000000000002</v>
       </c>
       <c r="G27" s="32">
-        <v>4.3890000000000002</v>
+        <v>2.7564000000000002</v>
       </c>
       <c r="H27" s="32">
-        <v>2.7564000000000002</v>
+        <v>3.4597000000000002</v>
       </c>
       <c r="I27" s="33">
-        <v>332.18060000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+        <v>320.54309999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="31"/>
       <c r="C28" s="32"/>
       <c r="D28" s="32"/>
@@ -13958,7 +14090,7 @@
       <c r="H28" s="32"/>
       <c r="I28" s="33"/>
     </row>
-    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="62" t="s">
         <v>32</v>
       </c>
@@ -13970,189 +14102,189 @@
       <c r="H29" s="63"/>
       <c r="I29" s="64"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="31" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="32">
-        <v>20.792200000000001</v>
+        <v>11.286099999999999</v>
       </c>
       <c r="D30" s="32">
-        <v>11.286099999999999</v>
+        <v>8.5932999999999993</v>
       </c>
       <c r="E30" s="32">
-        <v>8.5932999999999993</v>
+        <v>6.6547000000000001</v>
       </c>
       <c r="F30" s="32">
-        <v>6.6547000000000001</v>
+        <v>5.1981999999999999</v>
       </c>
       <c r="G30" s="32">
-        <v>5.1981999999999999</v>
+        <v>3.8534999999999999</v>
       </c>
       <c r="H30" s="32">
-        <v>3.8534999999999999</v>
+        <v>4.0476000000000001</v>
       </c>
       <c r="I30" s="33">
-        <v>260.64249999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+        <v>252.4357</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="32">
-        <v>19.951899999999998</v>
+        <v>11.7393</v>
       </c>
       <c r="D31" s="32">
-        <v>11.7393</v>
+        <v>8.7751000000000001</v>
       </c>
       <c r="E31" s="32">
-        <v>8.7751000000000001</v>
+        <v>6.6711</v>
       </c>
       <c r="F31" s="32">
-        <v>6.6711</v>
+        <v>5.5831999999999997</v>
       </c>
       <c r="G31" s="32">
-        <v>5.5831999999999997</v>
+        <v>3.5466000000000002</v>
       </c>
       <c r="H31" s="32">
-        <v>3.5466000000000002</v>
+        <v>4.1664000000000003</v>
       </c>
       <c r="I31" s="33">
-        <v>261.91340000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+        <v>254.2841</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="32">
-        <v>21.286100000000001</v>
+        <v>11.063000000000001</v>
       </c>
       <c r="D32" s="32">
-        <v>11.063000000000001</v>
+        <v>8.8963000000000001</v>
       </c>
       <c r="E32" s="32">
-        <v>8.8963000000000001</v>
+        <v>6.6332000000000004</v>
       </c>
       <c r="F32" s="32">
-        <v>6.6332000000000004</v>
+        <v>5.0351999999999997</v>
       </c>
       <c r="G32" s="32">
-        <v>5.0351999999999997</v>
+        <v>4.3135000000000003</v>
       </c>
       <c r="H32" s="32">
-        <v>4.3135000000000003</v>
+        <v>4.0545</v>
       </c>
       <c r="I32" s="33">
-        <v>262.30669999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+        <v>253.548</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="32">
-        <v>21.453700000000001</v>
+        <v>10.1144</v>
       </c>
       <c r="D33" s="32">
-        <v>10.1144</v>
+        <v>6.8185000000000002</v>
       </c>
       <c r="E33" s="32">
-        <v>6.8185000000000002</v>
+        <v>7.5838000000000001</v>
       </c>
       <c r="F33" s="32">
-        <v>7.5838000000000001</v>
+        <v>4.8856000000000002</v>
       </c>
       <c r="G33" s="32">
-        <v>4.8856000000000002</v>
+        <v>3.6046</v>
       </c>
       <c r="H33" s="32">
-        <v>3.6046</v>
+        <v>3.6335999999999999</v>
       </c>
       <c r="I33" s="33">
-        <v>249.90610000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+        <v>241.7422</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="32">
-        <v>19.4986</v>
+        <v>9.8995999999999995</v>
       </c>
       <c r="D34" s="32">
-        <v>9.8995999999999995</v>
+        <v>7.4158999999999997</v>
       </c>
       <c r="E34" s="32">
-        <v>7.4158999999999997</v>
+        <v>5.6147999999999998</v>
       </c>
       <c r="F34" s="32">
-        <v>5.6147999999999998</v>
+        <v>3.9249999999999998</v>
       </c>
       <c r="G34" s="32">
-        <v>3.9249999999999998</v>
+        <v>3.8592</v>
       </c>
       <c r="H34" s="32">
-        <v>3.8592</v>
+        <v>3.2067000000000001</v>
       </c>
       <c r="I34" s="33">
-        <v>246.15180000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+        <v>236.9554</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="31" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="32">
-        <v>21.833300000000001</v>
+        <v>11.944800000000001</v>
       </c>
       <c r="D35" s="32">
-        <v>11.944800000000001</v>
+        <v>8.0154999999999994</v>
       </c>
       <c r="E35" s="32">
-        <v>8.0154999999999994</v>
+        <v>6.5365000000000002</v>
       </c>
       <c r="F35" s="32">
-        <v>6.5365000000000002</v>
+        <v>4.5087999999999999</v>
       </c>
       <c r="G35" s="32">
-        <v>4.5087999999999999</v>
+        <v>3.6911</v>
       </c>
       <c r="H35" s="32">
-        <v>3.6911</v>
+        <v>4.3201999999999998</v>
       </c>
       <c r="I35" s="33">
-        <v>258.0763</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>251.96010000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="35">
-        <v>24.804600000000001</v>
+        <v>10.9206</v>
       </c>
       <c r="D36" s="35">
-        <v>10.9206</v>
+        <v>9.0473999999999997</v>
       </c>
       <c r="E36" s="35">
-        <v>9.0473999999999997</v>
+        <v>6.4358000000000004</v>
       </c>
       <c r="F36" s="35">
-        <v>6.4358000000000004</v>
+        <v>5.0989000000000004</v>
       </c>
       <c r="G36" s="35">
-        <v>5.0989000000000004</v>
+        <v>4.0114999999999998</v>
       </c>
       <c r="H36" s="35">
-        <v>4.0114999999999998</v>
+        <v>3.9363000000000001</v>
       </c>
       <c r="I36" s="36">
-        <v>269.99340000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>258.38099999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="54" t="s">
         <v>34</v>
       </c>
@@ -14164,7 +14296,7 @@
       <c r="H37" s="54"/>
       <c r="I37" s="54"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -14174,7 +14306,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -14204,17 +14336,17 @@
   <dimension ref="B1:I33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.42578125" customWidth="1"/>
-    <col min="3" max="9" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" customWidth="1"/>
+    <col min="3" max="9" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="55" t="s">
         <v>35</v>
       </c>
@@ -14226,7 +14358,7 @@
       <c r="H2" s="66"/>
       <c r="I2" s="67"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="37"/>
       <c r="C3" s="38" t="s">
         <v>19</v>
@@ -14250,7 +14382,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="29" t="s">
         <v>36</v>
       </c>
@@ -14262,345 +14394,345 @@
       <c r="H4" s="46"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="40" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="41">
-        <v>4.5137999999999998</v>
+        <v>4.0438999999999998</v>
       </c>
       <c r="D5" s="41">
-        <v>5.0039999999999996</v>
+        <v>4.2474999999999996</v>
       </c>
       <c r="E5" s="41">
-        <v>5.0018000000000002</v>
+        <v>3.8986000000000001</v>
       </c>
       <c r="F5" s="41">
-        <v>4.7289000000000003</v>
+        <v>4.6962999999999999</v>
       </c>
       <c r="G5" s="41">
-        <v>5.1580000000000004</v>
+        <v>4.7093999999999996</v>
       </c>
       <c r="H5" s="41">
-        <v>5.0720999999999998</v>
+        <v>4.0797999999999996</v>
       </c>
       <c r="I5" s="42">
-        <v>4.7572999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+        <v>4.1971999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="32">
-        <v>0.70950000000000002</v>
+        <v>1.1021000000000001</v>
       </c>
       <c r="D6" s="32">
-        <v>1.4341999999999999</v>
+        <v>1.1658999999999999</v>
       </c>
       <c r="E6" s="32">
-        <v>1.4381999999999999</v>
+        <v>0.95730000000000004</v>
       </c>
       <c r="F6" s="32">
-        <v>1.5616000000000001</v>
+        <v>1.0924</v>
       </c>
       <c r="G6" s="32">
-        <v>1.446</v>
+        <v>1.0822000000000001</v>
       </c>
       <c r="H6" s="32">
-        <v>1.4997</v>
+        <v>1.1146</v>
       </c>
       <c r="I6" s="33">
-        <v>1.1201000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+        <v>1.1131</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="32">
-        <v>5.28E-2</v>
+        <v>0.1704</v>
       </c>
       <c r="D7" s="32">
-        <v>5.67E-2</v>
+        <v>0.19209999999999999</v>
       </c>
       <c r="E7" s="32">
-        <v>4.82E-2</v>
+        <v>0.15840000000000001</v>
       </c>
       <c r="F7" s="32">
-        <v>5.9200000000000003E-2</v>
+        <v>0.18360000000000001</v>
       </c>
       <c r="G7" s="32">
-        <v>5.9499999999999997E-2</v>
+        <v>0.1799</v>
       </c>
       <c r="H7" s="32">
-        <v>6.1199999999999997E-2</v>
+        <v>0.17510000000000001</v>
       </c>
       <c r="I7" s="33">
-        <v>5.4800000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.17829999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="32">
-        <v>0.18820000000000001</v>
+        <v>0.14949999999999999</v>
       </c>
       <c r="D8" s="32">
-        <v>0.34129999999999999</v>
+        <v>0.23949999999999999</v>
       </c>
       <c r="E8" s="32">
-        <v>0.2266</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="F8" s="32">
-        <v>0.49109999999999998</v>
+        <v>0.32640000000000002</v>
       </c>
       <c r="G8" s="32">
-        <v>0.32219999999999999</v>
+        <v>0.2462</v>
       </c>
       <c r="H8" s="32">
-        <v>0.3448</v>
+        <v>0.3458</v>
       </c>
       <c r="I8" s="33">
-        <v>0.27089999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.21609999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="31" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="32">
-        <v>0.95499999999999996</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="D9" s="32">
-        <v>0.88670000000000004</v>
+        <v>0.3211</v>
       </c>
       <c r="E9" s="32">
-        <v>1.2285999999999999</v>
+        <v>0.48580000000000001</v>
       </c>
       <c r="F9" s="32">
-        <v>1.3148</v>
+        <v>1.5152000000000001</v>
       </c>
       <c r="G9" s="32">
-        <v>1.5185999999999999</v>
+        <v>0.54020000000000001</v>
       </c>
       <c r="H9" s="32">
-        <v>1.206</v>
+        <v>0.62580000000000002</v>
       </c>
       <c r="I9" s="33">
-        <v>1.0074000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.46060000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="32">
-        <v>9.11E-2</v>
+        <v>0.1202</v>
       </c>
       <c r="D10" s="32">
-        <v>0.14219999999999999</v>
+        <v>0.22559999999999999</v>
       </c>
       <c r="E10" s="32">
-        <v>0.14119999999999999</v>
+        <v>0.23019999999999999</v>
       </c>
       <c r="F10" s="32">
-        <v>0.1469</v>
+        <v>0.11360000000000001</v>
       </c>
       <c r="G10" s="32">
-        <v>0.1091</v>
+        <v>0.21</v>
       </c>
       <c r="H10" s="32">
-        <v>0.12770000000000001</v>
+        <v>0.17960000000000001</v>
       </c>
       <c r="I10" s="33">
-        <v>0.1171</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.17080000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="31" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="32">
-        <v>0.45619999999999999</v>
+        <v>0.54559999999999997</v>
       </c>
       <c r="D11" s="32">
-        <v>0.42030000000000001</v>
+        <v>0.6008</v>
       </c>
       <c r="E11" s="32">
-        <v>0.3962</v>
+        <v>0.34739999999999999</v>
       </c>
       <c r="F11" s="32">
-        <v>0.27660000000000001</v>
+        <v>0.36349999999999999</v>
       </c>
       <c r="G11" s="32">
-        <v>0.43</v>
+        <v>0.43120000000000003</v>
       </c>
       <c r="H11" s="32">
-        <v>0.30730000000000002</v>
+        <v>0.30420000000000003</v>
       </c>
       <c r="I11" s="33">
-        <v>0.42349999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.52569999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="32">
-        <v>0.43869999999999998</v>
+        <v>0.19739999999999999</v>
       </c>
       <c r="D12" s="32">
-        <v>0.51170000000000004</v>
+        <v>0.39250000000000002</v>
       </c>
       <c r="E12" s="32">
-        <v>0.41920000000000002</v>
+        <v>0.2447</v>
       </c>
       <c r="F12" s="32">
-        <v>0.18099999999999999</v>
+        <v>0.28849999999999998</v>
       </c>
       <c r="G12" s="32">
-        <v>0.52949999999999997</v>
+        <v>0.70979999999999999</v>
       </c>
       <c r="H12" s="32">
-        <v>0.64780000000000004</v>
+        <v>0.34460000000000002</v>
       </c>
       <c r="I12" s="33">
-        <v>0.46489999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.30470000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="31" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="32">
-        <v>0.13539999999999999</v>
+        <v>9.6799999999999997E-2</v>
       </c>
       <c r="D13" s="32">
-        <v>0.12640000000000001</v>
+        <v>9.2299999999999993E-2</v>
       </c>
       <c r="E13" s="32">
-        <v>0.1351</v>
+        <v>8.7800000000000003E-2</v>
       </c>
       <c r="F13" s="32">
-        <v>0.11990000000000001</v>
+        <v>0.1258</v>
       </c>
       <c r="G13" s="32">
-        <v>0.13769999999999999</v>
+        <v>0.11269999999999999</v>
       </c>
       <c r="H13" s="32">
-        <v>0.1033</v>
+        <v>0.1426</v>
       </c>
       <c r="I13" s="33">
-        <v>0.1303</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>9.8900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="31" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="32">
-        <v>0.39800000000000002</v>
+        <v>0.26790000000000003</v>
       </c>
       <c r="D14" s="32">
-        <v>0.40350000000000003</v>
+        <v>0.38169999999999998</v>
       </c>
       <c r="E14" s="32">
-        <v>0.26519999999999999</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="F14" s="32">
-        <v>0.25319999999999998</v>
+        <v>0.2298</v>
       </c>
       <c r="G14" s="32">
-        <v>0.25740000000000002</v>
+        <v>0.29210000000000003</v>
       </c>
       <c r="H14" s="32">
-        <v>0.13730000000000001</v>
+        <v>0.33119999999999999</v>
       </c>
       <c r="I14" s="33">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.31119999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="31" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="32">
-        <v>0.19040000000000001</v>
+        <v>5.1900000000000002E-2</v>
       </c>
       <c r="D15" s="32">
-        <v>7.5300000000000006E-2</v>
+        <v>5.4899999999999997E-2</v>
       </c>
       <c r="E15" s="32">
-        <v>0.15820000000000001</v>
+        <v>8.2699999999999996E-2</v>
       </c>
       <c r="F15" s="32">
-        <v>6.13E-2</v>
+        <v>0.1163</v>
       </c>
       <c r="G15" s="32">
-        <v>7.3200000000000001E-2</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="H15" s="32">
-        <v>0.11849999999999999</v>
+        <v>5.0500000000000003E-2</v>
       </c>
       <c r="I15" s="33">
-        <v>0.13370000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+        <v>5.8599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="32">
-        <v>0.80589999999999995</v>
+        <v>0.79069999999999996</v>
       </c>
       <c r="D16" s="32">
-        <v>0.48020000000000002</v>
+        <v>0.47070000000000001</v>
       </c>
       <c r="E16" s="32">
-        <v>0.48110000000000003</v>
+        <v>0.52669999999999995</v>
       </c>
       <c r="F16" s="32">
-        <v>0.21</v>
+        <v>0.1971</v>
       </c>
       <c r="G16" s="32">
-        <v>0.2447</v>
+        <v>0.68630000000000002</v>
       </c>
       <c r="H16" s="32">
-        <v>0.38800000000000001</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="I16" s="33">
-        <v>0.59719999999999995</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="32">
-        <v>9.2700000000000005E-2</v>
+        <v>0.1206</v>
       </c>
       <c r="D17" s="32">
-        <v>0.12540000000000001</v>
+        <v>0.1104</v>
       </c>
       <c r="E17" s="32">
-        <v>6.4000000000000001E-2</v>
+        <v>0.13059999999999999</v>
       </c>
       <c r="F17" s="32">
-        <v>5.3499999999999999E-2</v>
+        <v>0.14410000000000001</v>
       </c>
       <c r="G17" s="32">
-        <v>3.0099999999999998E-2</v>
+        <v>0.1527</v>
       </c>
       <c r="H17" s="32">
-        <v>0.1305</v>
+        <v>0.1328</v>
       </c>
       <c r="I17" s="33">
-        <v>9.8599999999999993E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.1211</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="43"/>
       <c r="C18" s="44"/>
       <c r="D18" s="44"/>
@@ -14610,7 +14742,7 @@
       <c r="H18" s="44"/>
       <c r="I18" s="45"/>
     </row>
-    <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="62" t="s">
         <v>36</v>
       </c>
@@ -14622,345 +14754,345 @@
       <c r="H19" s="63"/>
       <c r="I19" s="64"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="40" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="41">
-        <v>273.67910000000001</v>
+        <v>266.11270000000002</v>
       </c>
       <c r="D20" s="41">
-        <v>271.63900000000001</v>
+        <v>262.89229999999998</v>
       </c>
       <c r="E20" s="41">
-        <v>262.37830000000002</v>
+        <v>253.87440000000001</v>
       </c>
       <c r="F20" s="41">
-        <v>258.69819999999999</v>
+        <v>253.12039999999999</v>
       </c>
       <c r="G20" s="41">
-        <v>271.86020000000002</v>
+        <v>265.8569</v>
       </c>
       <c r="H20" s="41">
-        <v>276.87759999999997</v>
+        <v>264.16149999999999</v>
       </c>
       <c r="I20" s="42">
-        <v>271.52969999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+        <v>263.44569999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="32">
-        <v>74.219099999999997</v>
+        <v>71.886499999999998</v>
       </c>
       <c r="D21" s="32">
-        <v>87.811800000000005</v>
+        <v>84.264200000000002</v>
       </c>
       <c r="E21" s="32">
-        <v>99.911500000000004</v>
+        <v>94.576700000000002</v>
       </c>
       <c r="F21" s="32">
-        <v>96.698099999999997</v>
+        <v>92.145899999999997</v>
       </c>
       <c r="G21" s="32">
-        <v>86.847399999999993</v>
+        <v>83.198499999999996</v>
       </c>
       <c r="H21" s="32">
-        <v>84.8386</v>
+        <v>80.682000000000002</v>
       </c>
       <c r="I21" s="33">
-        <v>82.787300000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+        <v>79.581199999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="32">
-        <v>6.7531999999999996</v>
+        <v>6.7106000000000003</v>
       </c>
       <c r="D22" s="32">
-        <v>7.8808999999999996</v>
+        <v>7.7443999999999997</v>
       </c>
       <c r="E22" s="32">
-        <v>6.0449999999999999</v>
+        <v>5.9869000000000003</v>
       </c>
       <c r="F22" s="32">
-        <v>7.4863</v>
+        <v>7.3277999999999999</v>
       </c>
       <c r="G22" s="32">
-        <v>7.0091000000000001</v>
+        <v>6.9134000000000002</v>
       </c>
       <c r="H22" s="32">
-        <v>7.5183999999999997</v>
+        <v>7.2373000000000003</v>
       </c>
       <c r="I22" s="33">
-        <v>7.1712999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+        <v>7.0766999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="32">
-        <v>19.516300000000001</v>
+        <v>18.351500000000001</v>
       </c>
       <c r="D23" s="32">
-        <v>23.116199999999999</v>
+        <v>22.011800000000001</v>
       </c>
       <c r="E23" s="32">
-        <v>23.030200000000001</v>
+        <v>22.214200000000002</v>
       </c>
       <c r="F23" s="32">
-        <v>21.474699999999999</v>
+        <v>21.004000000000001</v>
       </c>
       <c r="G23" s="32">
-        <v>22.228000000000002</v>
+        <v>21.384499999999999</v>
       </c>
       <c r="H23" s="32">
-        <v>28.081600000000002</v>
+        <v>26.547899999999998</v>
       </c>
       <c r="I23" s="33">
-        <v>21.609100000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+        <v>20.52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="31" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="32">
-        <v>24.472100000000001</v>
+        <v>24.290900000000001</v>
       </c>
       <c r="D24" s="32">
-        <v>18.319099999999999</v>
+        <v>18.119</v>
       </c>
       <c r="E24" s="32">
-        <v>18.7911</v>
+        <v>19.139900000000001</v>
       </c>
       <c r="F24" s="32">
-        <v>20.311599999999999</v>
+        <v>23.799600000000002</v>
       </c>
       <c r="G24" s="32">
-        <v>23.415099999999999</v>
+        <v>23.5745</v>
       </c>
       <c r="H24" s="32">
-        <v>25.052900000000001</v>
+        <v>24.9877</v>
       </c>
       <c r="I24" s="33">
-        <v>21.761700000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+        <v>21.7989</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="32">
-        <v>15.9543</v>
+        <v>15.334199999999999</v>
       </c>
       <c r="D25" s="32">
-        <v>16.167300000000001</v>
+        <v>15.6305</v>
       </c>
       <c r="E25" s="32">
-        <v>14.915100000000001</v>
+        <v>14.507400000000001</v>
       </c>
       <c r="F25" s="32">
-        <v>19.460999999999999</v>
+        <v>18.5304</v>
       </c>
       <c r="G25" s="32">
-        <v>15.748799999999999</v>
+        <v>15.2112</v>
       </c>
       <c r="H25" s="32">
-        <v>18.5078</v>
+        <v>17.421399999999998</v>
       </c>
       <c r="I25" s="33">
-        <v>16.219799999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+        <v>15.611800000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="31" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="32">
-        <v>26.116599999999998</v>
+        <v>25.829000000000001</v>
       </c>
       <c r="D26" s="32">
-        <v>26.243500000000001</v>
+        <v>25.952000000000002</v>
       </c>
       <c r="E26" s="32">
-        <v>20.054600000000001</v>
+        <v>19.4451</v>
       </c>
       <c r="F26" s="32">
-        <v>16.668900000000001</v>
+        <v>16.398</v>
       </c>
       <c r="G26" s="32">
-        <v>25.357700000000001</v>
+        <v>24.579599999999999</v>
       </c>
       <c r="H26" s="32">
-        <v>15.832100000000001</v>
+        <v>15.259499999999999</v>
       </c>
       <c r="I26" s="33">
-        <v>24.807600000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+        <v>24.4587</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="32">
-        <v>32.602200000000003</v>
+        <v>31.003499999999999</v>
       </c>
       <c r="D27" s="32">
-        <v>32.613199999999999</v>
+        <v>31.392600000000002</v>
       </c>
       <c r="E27" s="32">
-        <v>24.673500000000001</v>
+        <v>23.601199999999999</v>
       </c>
       <c r="F27" s="32">
-        <v>31.1966</v>
+        <v>29.8001</v>
       </c>
       <c r="G27" s="32">
-        <v>37.719099999999997</v>
+        <v>37.241399999999999</v>
       </c>
       <c r="H27" s="32">
-        <v>44.152700000000003</v>
+        <v>40.8078</v>
       </c>
       <c r="I27" s="33">
-        <v>32.79</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+        <v>31.344200000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="31" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="32">
-        <v>7.4682000000000004</v>
+        <v>7.1302000000000003</v>
       </c>
       <c r="D28" s="32">
-        <v>7.3689</v>
+        <v>6.9105999999999996</v>
       </c>
       <c r="E28" s="32">
-        <v>6.5911</v>
+        <v>6.2911000000000001</v>
       </c>
       <c r="F28" s="32">
-        <v>7.2365000000000004</v>
+        <v>6.9634999999999998</v>
       </c>
       <c r="G28" s="32">
-        <v>5.7149999999999999</v>
+        <v>5.5921000000000003</v>
       </c>
       <c r="H28" s="32">
-        <v>6.7792000000000003</v>
+        <v>6.5476999999999999</v>
       </c>
       <c r="I28" s="33">
-        <v>7.2412000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+        <v>6.8836000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="31" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="32">
-        <v>19.470500000000001</v>
+        <v>18.876899999999999</v>
       </c>
       <c r="D29" s="32">
-        <v>17.2121</v>
+        <v>16.8249</v>
       </c>
       <c r="E29" s="32">
-        <v>13.086</v>
+        <v>13.1732</v>
       </c>
       <c r="F29" s="32">
-        <v>14.2826</v>
+        <v>13.7226</v>
       </c>
       <c r="G29" s="32">
-        <v>15.402100000000001</v>
+        <v>14.9857</v>
       </c>
       <c r="H29" s="32">
-        <v>18.353300000000001</v>
+        <v>17.751799999999999</v>
       </c>
       <c r="I29" s="33">
-        <v>17.763300000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+        <v>17.297499999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="31" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="32">
-        <v>6.7157999999999998</v>
+        <v>6.4077000000000002</v>
       </c>
       <c r="D30" s="32">
-        <v>2.3732000000000002</v>
+        <v>2.3260999999999998</v>
       </c>
       <c r="E30" s="32">
-        <v>3.6349</v>
+        <v>3.6293000000000002</v>
       </c>
       <c r="F30" s="32">
-        <v>1.8635999999999999</v>
+        <v>2.0642</v>
       </c>
       <c r="G30" s="32">
-        <v>3.0316999999999998</v>
+        <v>3.0169999999999999</v>
       </c>
       <c r="H30" s="32">
-        <v>2.9573999999999998</v>
+        <v>2.8727999999999998</v>
       </c>
       <c r="I30" s="33">
-        <v>4.4377000000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+        <v>4.2880000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="32">
-        <v>30.538699999999999</v>
+        <v>30.777899999999999</v>
       </c>
       <c r="D31" s="32">
-        <v>22.328299999999999</v>
+        <v>21.909099999999999</v>
       </c>
       <c r="E31" s="32">
-        <v>21.950700000000001</v>
+        <v>21.879899999999999</v>
       </c>
       <c r="F31" s="32">
-        <v>12.428000000000001</v>
+        <v>12.012499999999999</v>
       </c>
       <c r="G31" s="32">
-        <v>18.895600000000002</v>
+        <v>19.9298</v>
       </c>
       <c r="H31" s="32">
-        <v>14.2805</v>
+        <v>14.0641</v>
       </c>
       <c r="I31" s="33">
-        <v>24.977799999999998</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>24.961400000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="34" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="35">
-        <v>9.8498000000000001</v>
+        <v>9.5104000000000006</v>
       </c>
       <c r="D32" s="35">
-        <v>10.206300000000001</v>
+        <v>9.8079000000000001</v>
       </c>
       <c r="E32" s="35">
-        <v>9.6963000000000008</v>
+        <v>9.4313000000000002</v>
       </c>
       <c r="F32" s="35">
-        <v>9.5862999999999996</v>
+        <v>9.3466000000000005</v>
       </c>
       <c r="G32" s="35">
-        <v>10.4838</v>
+        <v>10.2232</v>
       </c>
       <c r="H32" s="35">
-        <v>10.517899999999999</v>
+        <v>9.9777000000000005</v>
       </c>
       <c r="I32" s="36">
-        <v>10.012600000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9.6576000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="68" t="s">
         <v>38</v>
       </c>

</xml_diff>